<commit_message>
Cigna flow Colmpleted Testing Remaining
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>https://www.aetna.com/dsepublic/#/contentPage?page=providerSearchLanding&amp;site_id=dse&amp;language=en</t>
+  </si>
+  <si>
+    <t>URL_Cigna</t>
+  </si>
+  <si>
+    <t>Cigna Website URL</t>
+  </si>
+  <si>
+    <t>https://hcpdirectory.cigna.com/web/public/consumer/directory/search?consumerCode=HDC001</t>
   </si>
 </sst>
 </file>
@@ -562,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -621,87 +630,97 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>54</v>
+      <c r="A10" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1679,6 +1698,7 @@
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Config file now has flexible run option & Blue Cross Blue Shield WF added
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="Constants" sheetId="2" r:id="rId2"/>
+    <sheet name="States" sheetId="3" r:id="rId2"/>
+    <sheet name="Constants" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -151,45 +152,6 @@
     <t>Maximum retry attempts for certain workflows</t>
   </si>
   <si>
-    <t>Email_From</t>
-  </si>
-  <si>
-    <t>Sender's email address</t>
-  </si>
-  <si>
-    <t>Email_To</t>
-  </si>
-  <si>
-    <t>email address for the receiving party\parties</t>
-  </si>
-  <si>
-    <t>Email_Cc</t>
-  </si>
-  <si>
-    <t>email address for the receiving party\parties for cc</t>
-  </si>
-  <si>
-    <t>ErrorEmail_To</t>
-  </si>
-  <si>
-    <t>Developer's email Address</t>
-  </si>
-  <si>
-    <t>ErrorEmail_Cc</t>
-  </si>
-  <si>
-    <t>Solution Architect's Email Address</t>
-  </si>
-  <si>
-    <t>SME Email Address or the Team's DL</t>
-  </si>
-  <si>
-    <t>Email_SME</t>
-  </si>
-  <si>
-    <t>WC_HG</t>
-  </si>
-  <si>
     <t>URL_Aetna</t>
   </si>
   <si>
@@ -209,13 +171,364 @@
   </si>
   <si>
     <t>https://hcpdirectory.cigna.com/web/public/consumer/directory/search?consumerCode=HDC001</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>ALABAMA</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>ALASKA</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>ARIZONA</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>ARKANSAS</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CALIFORNIA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>COLORADO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>CONNECTICUT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DELAWARE</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>HAWAII</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IDAHO</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>ILLINOIS</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>INDIANA</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>IOWA</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KANSAS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>KENTUCKY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>LOUISIANA</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MAINE</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MARYLAND</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MASSACHUSETTS</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MICHIGAN</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MINNESOTA</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MISSOURI</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>MONTANA</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NEBRASKA</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NEVADA</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NEW HAMPSHIRE</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NEW JERSEY</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NEW MEXICO</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>NORTH DAKOTA</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OHIO</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OKLAHOMA</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>OREGON</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PENNSYLVANIA</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>RHODE ISLAND</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SOUTH CAROLINA</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SOUTH DAKOTA</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TENNESSEE</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>UTAH</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>VERMONT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VIRGINIA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WASHINGTON</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WEST VIRGINIA</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WISCONSIN</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>WYOMING</t>
+  </si>
+  <si>
+    <t>Aetna</t>
+  </si>
+  <si>
+    <t>Cigna</t>
+  </si>
+  <si>
+    <t>Blue Cross Blue Shield</t>
+  </si>
+  <si>
+    <t>Coventry Health Care</t>
+  </si>
+  <si>
+    <t>First Health (Coventry Health Care)</t>
+  </si>
+  <si>
+    <t>PPO</t>
+  </si>
+  <si>
+    <t>PHCS</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Rest</t>
+  </si>
+  <si>
+    <t>Anthem</t>
+  </si>
+  <si>
+    <t>Y or N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Delta Dental</t>
+  </si>
+  <si>
+    <t>URL_BCBS</t>
+  </si>
+  <si>
+    <t>https://provider.bcbs.com/app/public/#/one/city=&amp;state=&amp;postalCode=&amp;country=&amp;insurerCode=BCBSA_I&amp;brandCode=BCBSANDHF&amp;alphaPrefix=&amp;bcbsaProductId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -242,15 +555,22 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,32 +590,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 4" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -571,17 +928,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -589,10 +946,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
@@ -621,107 +978,166 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>165</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="2" t="s">
-        <v>44</v>
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>152</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="2" t="s">
-        <v>48</v>
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="2" t="s">
-        <v>50</v>
+      <c r="A9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="2" t="s">
-        <v>52</v>
+      <c r="A10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1693,23 +2109,468 @@
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="B6:B15">
+    <cfRule type="expression" dxfId="3" priority="11">
+      <formula>$B6="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="12">
+      <formula>$B6="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$B16="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$B16="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Blue Cross Blue Shield WF added
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -13,14 +13,15 @@
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="Constants" sheetId="2" r:id="rId2"/>
+    <sheet name="States" sheetId="3" r:id="rId2"/>
+    <sheet name="Constants" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -151,45 +152,6 @@
     <t>Maximum retry attempts for certain workflows</t>
   </si>
   <si>
-    <t>Email_From</t>
-  </si>
-  <si>
-    <t>Sender's email address</t>
-  </si>
-  <si>
-    <t>Email_To</t>
-  </si>
-  <si>
-    <t>email address for the receiving party\parties</t>
-  </si>
-  <si>
-    <t>Email_Cc</t>
-  </si>
-  <si>
-    <t>email address for the receiving party\parties for cc</t>
-  </si>
-  <si>
-    <t>ErrorEmail_To</t>
-  </si>
-  <si>
-    <t>Developer's email Address</t>
-  </si>
-  <si>
-    <t>ErrorEmail_Cc</t>
-  </si>
-  <si>
-    <t>Solution Architect's Email Address</t>
-  </si>
-  <si>
-    <t>SME Email Address or the Team's DL</t>
-  </si>
-  <si>
-    <t>Email_SME</t>
-  </si>
-  <si>
-    <t>WC_HG</t>
-  </si>
-  <si>
     <t>URL_Aetna</t>
   </si>
   <si>
@@ -209,13 +171,364 @@
   </si>
   <si>
     <t>https://hcpdirectory.cigna.com/web/public/consumer/directory/search?consumerCode=HDC001</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>ALABAMA</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>ALASKA</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>ARIZONA</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>ARKANSAS</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CALIFORNIA</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>COLORADO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>CONNECTICUT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DELAWARE</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>FLORIDA</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>GEORGIA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>HAWAII</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IDAHO</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>ILLINOIS</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>INDIANA</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>IOWA</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>KANSAS</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>KENTUCKY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>LOUISIANA</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MAINE</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>MARYLAND</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MASSACHUSETTS</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MICHIGAN</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MINNESOTA</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MISSISSIPPI</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MISSOURI</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>MONTANA</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NEBRASKA</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NEVADA</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NEW HAMPSHIRE</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NEW JERSEY</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NEW MEXICO</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NORTH CAROLINA</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>NORTH DAKOTA</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OHIO</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OKLAHOMA</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>OREGON</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PENNSYLVANIA</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>RHODE ISLAND</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SOUTH CAROLINA</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SOUTH DAKOTA</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TENNESSEE</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>TEXAS</t>
+  </si>
+  <si>
+    <t>UT</t>
+  </si>
+  <si>
+    <t>UTAH</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>VERMONT</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VIRGINIA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>WASHINGTON</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WEST VIRGINIA</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WISCONSIN</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>WYOMING</t>
+  </si>
+  <si>
+    <t>Aetna</t>
+  </si>
+  <si>
+    <t>Cigna</t>
+  </si>
+  <si>
+    <t>Blue Cross Blue Shield</t>
+  </si>
+  <si>
+    <t>Coventry Health Care</t>
+  </si>
+  <si>
+    <t>First Health (Coventry Health Care)</t>
+  </si>
+  <si>
+    <t>PPO</t>
+  </si>
+  <si>
+    <t>PHCS</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Rest</t>
+  </si>
+  <si>
+    <t>Anthem</t>
+  </si>
+  <si>
+    <t>Y or N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Delta Dental</t>
+  </si>
+  <si>
+    <t>URL_BCBS</t>
+  </si>
+  <si>
+    <t>https://provider.bcbs.com/app/public/#/one/city=&amp;state=&amp;postalCode=&amp;country=&amp;insurerCode=BCBSA_I&amp;brandCode=BCBSANDHF&amp;alphaPrefix=&amp;bcbsaProductId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -242,15 +555,22 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -270,32 +590,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 4" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -571,17 +928,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -589,10 +946,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
@@ -621,107 +978,166 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>165</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="2" t="s">
-        <v>44</v>
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>152</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="2" t="s">
-        <v>48</v>
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="2" t="s">
-        <v>50</v>
+      <c r="A9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="2" t="s">
-        <v>52</v>
+      <c r="A10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1693,23 +2109,468 @@
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <conditionalFormatting sqref="B6:B15">
+    <cfRule type="expression" dxfId="3" priority="11">
+      <formula>$B6="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="12">
+      <formula>$B6="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$B16="N"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$B16="Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cigna Development and Testing Done
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -528,7 +528,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -572,6 +572,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -596,14 +603,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,6 +622,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +633,35 @@
     <cellStyle name="Normal 3" xfId="1"/>
     <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -937,8 +975,8 @@
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -946,10 +984,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
@@ -980,10 +1018,10 @@
       <c r="A2" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -991,10 +1029,10 @@
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1002,10 +1040,10 @@
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1013,128 +1051,128 @@
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C8" s="10" t="s">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="9" t="s">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B10" s="9" t="s">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B11" s="9" t="s">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="9" t="s">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="9" t="s">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B14" s="9" t="s">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>159</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2110,23 +2148,16 @@
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="B6:B15">
-    <cfRule type="expression" dxfId="3" priority="11">
+  <conditionalFormatting sqref="A6:A16">
+    <cfRule type="expression" dxfId="5" priority="11">
       <formula>$B6="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="4" priority="12">
       <formula>$B6="Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$B16="N"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$B16="Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Anthem WF added before testing
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="States" sheetId="3" r:id="rId2"/>
     <sheet name="Constants" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="171">
   <si>
     <t>Name</t>
   </si>
@@ -176,306 +176,156 @@
     <t>AL</t>
   </si>
   <si>
-    <t>ALABAMA</t>
-  </si>
-  <si>
     <t>AK</t>
   </si>
   <si>
-    <t>ALASKA</t>
-  </si>
-  <si>
     <t>AZ</t>
   </si>
   <si>
-    <t>ARIZONA</t>
-  </si>
-  <si>
     <t>AR</t>
   </si>
   <si>
-    <t>ARKANSAS</t>
-  </si>
-  <si>
     <t>CA</t>
   </si>
   <si>
-    <t>CALIFORNIA</t>
-  </si>
-  <si>
     <t>CO</t>
   </si>
   <si>
-    <t>COLORADO</t>
-  </si>
-  <si>
     <t>CT</t>
   </si>
   <si>
-    <t>CONNECTICUT</t>
-  </si>
-  <si>
     <t>DE</t>
   </si>
   <si>
-    <t>DELAWARE</t>
-  </si>
-  <si>
     <t>DC</t>
   </si>
   <si>
     <t>FL</t>
   </si>
   <si>
-    <t>FLORIDA</t>
-  </si>
-  <si>
     <t>GA</t>
   </si>
   <si>
-    <t>GEORGIA</t>
-  </si>
-  <si>
     <t>HI</t>
   </si>
   <si>
-    <t>HAWAII</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
-    <t>IDAHO</t>
-  </si>
-  <si>
     <t>IL</t>
   </si>
   <si>
-    <t>ILLINOIS</t>
-  </si>
-  <si>
     <t>IN</t>
   </si>
   <si>
-    <t>INDIANA</t>
-  </si>
-  <si>
     <t>IA</t>
   </si>
   <si>
-    <t>IOWA</t>
-  </si>
-  <si>
     <t>KS</t>
   </si>
   <si>
-    <t>KANSAS</t>
-  </si>
-  <si>
     <t>KY</t>
   </si>
   <si>
-    <t>KENTUCKY</t>
-  </si>
-  <si>
     <t>LA</t>
   </si>
   <si>
-    <t>LOUISIANA</t>
-  </si>
-  <si>
     <t>ME</t>
   </si>
   <si>
-    <t>MAINE</t>
-  </si>
-  <si>
     <t>MD</t>
   </si>
   <si>
-    <t>MARYLAND</t>
-  </si>
-  <si>
     <t>MA</t>
   </si>
   <si>
-    <t>MASSACHUSETTS</t>
-  </si>
-  <si>
     <t>MI</t>
   </si>
   <si>
-    <t>MICHIGAN</t>
-  </si>
-  <si>
     <t>MN</t>
   </si>
   <si>
-    <t>MINNESOTA</t>
-  </si>
-  <si>
     <t>MS</t>
   </si>
   <si>
-    <t>MISSISSIPPI</t>
-  </si>
-  <si>
     <t>MO</t>
   </si>
   <si>
-    <t>MISSOURI</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
-    <t>MONTANA</t>
-  </si>
-  <si>
     <t>NE</t>
   </si>
   <si>
-    <t>NEBRASKA</t>
-  </si>
-  <si>
     <t>NV</t>
   </si>
   <si>
-    <t>NEVADA</t>
-  </si>
-  <si>
     <t>NH</t>
   </si>
   <si>
-    <t>NEW HAMPSHIRE</t>
-  </si>
-  <si>
     <t>NJ</t>
   </si>
   <si>
-    <t>NEW JERSEY</t>
-  </si>
-  <si>
     <t>NM</t>
   </si>
   <si>
-    <t>NEW MEXICO</t>
-  </si>
-  <si>
     <t>NY</t>
   </si>
   <si>
-    <t>NEW YORK</t>
-  </si>
-  <si>
     <t>NC</t>
   </si>
   <si>
-    <t>NORTH CAROLINA</t>
-  </si>
-  <si>
     <t>ND</t>
   </si>
   <si>
-    <t>NORTH DAKOTA</t>
-  </si>
-  <si>
     <t>OH</t>
   </si>
   <si>
-    <t>OHIO</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>OKLAHOMA</t>
-  </si>
-  <si>
     <t>OR</t>
   </si>
   <si>
-    <t>OREGON</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
-    <t>PENNSYLVANIA</t>
-  </si>
-  <si>
     <t>RI</t>
   </si>
   <si>
-    <t>RHODE ISLAND</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
-    <t>SOUTH CAROLINA</t>
-  </si>
-  <si>
     <t>SD</t>
   </si>
   <si>
-    <t>SOUTH DAKOTA</t>
-  </si>
-  <si>
     <t>TN</t>
   </si>
   <si>
-    <t>TENNESSEE</t>
-  </si>
-  <si>
     <t>TX</t>
   </si>
   <si>
-    <t>TEXAS</t>
-  </si>
-  <si>
     <t>UT</t>
   </si>
   <si>
-    <t>UTAH</t>
-  </si>
-  <si>
     <t>VT</t>
   </si>
   <si>
-    <t>VERMONT</t>
-  </si>
-  <si>
     <t>VA</t>
   </si>
   <si>
-    <t>VIRGINIA</t>
-  </si>
-  <si>
     <t>WA</t>
   </si>
   <si>
-    <t>WASHINGTON</t>
-  </si>
-  <si>
     <t>WV</t>
   </si>
   <si>
-    <t>WEST VIRGINIA</t>
-  </si>
-  <si>
     <t>WI</t>
   </si>
   <si>
-    <t>WISCONSIN</t>
-  </si>
-  <si>
     <t>WY</t>
   </si>
   <si>
-    <t>WYOMING</t>
-  </si>
-  <si>
     <t>Aetna</t>
   </si>
   <si>
@@ -522,6 +372,168 @@
   </si>
   <si>
     <t>https://provider.bcbs.com/app/public/#/one/city=&amp;state=&amp;postalCode=&amp;country=&amp;insurerCode=BCBSA_I&amp;brandCode=BCBSANDHF&amp;alphaPrefix=&amp;bcbsaProductId</t>
+  </si>
+  <si>
+    <t>URL_Anthem</t>
+  </si>
+  <si>
+    <t>https://www.anthem.com/health-insurance/providerreimagine-directory/searchcriteria?brand=ABCBS</t>
+  </si>
+  <si>
+    <t>Anthem Website URL</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>Dc</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
   </si>
 </sst>
 </file>
@@ -633,49 +645,7 @@
     <cellStyle name="Normal 3" xfId="1"/>
     <cellStyle name="Normal 4" xfId="3"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -966,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1016,10 +986,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>45</v>
@@ -1049,149 +1019,159 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B6" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>161</v>
+        <v>113</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>156</v>
+        <v>105</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>157</v>
+        <v>106</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>159</v>
+        <v>108</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>164</v>
+        <v>109</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>113</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2147,13 +2127,14 @@
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A6:A16">
-    <cfRule type="expression" dxfId="5" priority="11">
-      <formula>$B6="N"</formula>
+  <conditionalFormatting sqref="A7:A17">
+    <cfRule type="expression" dxfId="1" priority="11">
+      <formula>$B7="N"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="12">
-      <formula>$B6="Y"</formula>
+    <cfRule type="expression" dxfId="0" priority="12">
+      <formula>$B7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2165,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,407 +2168,407 @@
         <v>50</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>61</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>70</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>84</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>92</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>100</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>117</v>
+        <v>84</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>135</v>
+        <v>93</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cigna Bug Fixing and Added Multiplan WF
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1044,7 +1044,7 @@
         <v>101</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>111</v>
@@ -1055,7 +1055,7 @@
         <v>102</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>111</v>
@@ -1077,7 +1077,7 @@
         <v>110</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>111</v>
@@ -2146,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
County validation removed from Cigna, Anthem selector fixed, Multiplan Development and First Set of Testing Done
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="173">
   <si>
     <t>Name</t>
   </si>
@@ -534,6 +534,12 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>URL_Multiplan</t>
+  </si>
+  <si>
+    <t>https://www.multiplan.com/webcenter/portal/ProviderSearch?_afrLoop=4494409455183375&amp;_afrWindowMode=2&amp;Adf-Window-Id=g6y1unwep&amp;_afrFS=16&amp;_afrMT=screen&amp;_afrMFW=1366&amp;_afrMFH=576&amp;_afrMFDW=1366&amp;_afrMFDH=768&amp;_afrMFC=8&amp;_afrMFCI=0&amp;_afrMFM=0&amp;_afrMFR=96&amp;_afrMFG=0&amp;_afrMFS=0&amp;_afrMFO=0</t>
   </si>
 </sst>
 </file>
@@ -936,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1030,40 +1036,38 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B7" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>113</v>
@@ -1074,7 +1078,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>113</v>
@@ -1085,10 +1089,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>111</v>
@@ -1096,7 +1100,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>113</v>
@@ -1107,7 +1111,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>113</v>
@@ -1118,7 +1122,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>113</v>
@@ -1129,7 +1133,7 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>113</v>
@@ -1140,7 +1144,7 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>113</v>
@@ -1149,29 +1153,42 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C17" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2128,13 +2145,14 @@
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A7:A17">
+  <conditionalFormatting sqref="A8:A18">
     <cfRule type="expression" dxfId="1" priority="11">
-      <formula>$B7="N"</formula>
+      <formula>$B8="N"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="12">
-      <formula>$B7="Y"</formula>
+      <formula>$B8="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Delta Dental WF Tested
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="177">
   <si>
     <t>Name</t>
   </si>
@@ -540,6 +540,18 @@
   </si>
   <si>
     <t>https://www.multiplan.com/webcenter/portal/ProviderSearch?_afrLoop=4494409455183375&amp;_afrWindowMode=2&amp;Adf-Window-Id=g6y1unwep&amp;_afrFS=16&amp;_afrMT=screen&amp;_afrMFW=1366&amp;_afrMFH=576&amp;_afrMFDW=1366&amp;_afrMFDH=768&amp;_afrMFC=8&amp;_afrMFCI=0&amp;_afrMFM=0&amp;_afrMFR=96&amp;_afrMFG=0&amp;_afrMFS=0&amp;_afrMFO=0</t>
+  </si>
+  <si>
+    <t>Multiplan Website URL</t>
+  </si>
+  <si>
+    <t>Delta Dental Website</t>
+  </si>
+  <si>
+    <t>URL_Delta</t>
+  </si>
+  <si>
+    <t>https://www.deltadentalins.com/find-a-dentist/directory-results/?d=enterprise&amp;network=2ppo&amp;location=2064%20Baldwin%20St;%20Ste%20A;%20Jenison;%20MI%2049428&amp;distance=15&amp;lat=42.9068881&amp;long=-85.8330607&amp;free_text=Vurugonda%20Anupama&amp;sort_field=relevance&amp;sort_order=asc&amp;isBookmarkedURL=false&amp;page=1</t>
   </si>
 </sst>
 </file>
@@ -942,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1041,44 +1053,46 @@
       <c r="B6" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B8" s="7">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>113</v>
@@ -1089,10 +1103,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>111</v>
@@ -1100,7 +1114,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>113</v>
@@ -1111,7 +1125,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>113</v>
@@ -1122,7 +1136,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>113</v>
@@ -1133,10 +1147,10 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>111</v>
@@ -1144,10 +1158,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>111</v>
@@ -1155,7 +1169,7 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>113</v>
@@ -1166,7 +1180,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>113</v>
@@ -1175,7 +1189,17 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2146,13 +2170,14 @@
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A8:A18">
+  <conditionalFormatting sqref="A9:A19">
     <cfRule type="expression" dxfId="1" priority="11">
-      <formula>$B8="N"</formula>
+      <formula>$B9="N"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="12">
-      <formula>$B8="Y"</formula>
+      <formula>$B9="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Anthem completed and Tested
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z990"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1117,7 @@
         <v>110</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>111</v>
@@ -1150,7 +1150,7 @@
         <v>106</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>111</v>
@@ -1161,7 +1161,7 @@
         <v>107</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>111</v>
@@ -1194,7 +1194,7 @@
         <v>114</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>111</v>

</xml_diff>

<commit_message>
First Health Coventry Added and bug fixed
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="184">
   <si>
     <t>Name</t>
   </si>
@@ -545,13 +545,34 @@
     <t>Multiplan Website URL</t>
   </si>
   <si>
-    <t>Delta Dental Website</t>
-  </si>
-  <si>
     <t>URL_Delta</t>
   </si>
   <si>
     <t>https://www.deltadentalins.com/find-a-dentist/directory-results/?d=enterprise&amp;network=2ppo&amp;location=2064%20Baldwin%20St;%20Ste%20A;%20Jenison;%20MI%2049428&amp;distance=15&amp;lat=42.9068881&amp;long=-85.8330607&amp;free_text=Vurugonda%20Anupama&amp;sort_field=relevance&amp;sort_order=asc&amp;isBookmarkedURL=false&amp;page=1</t>
+  </si>
+  <si>
+    <t>URL_Coventry</t>
+  </si>
+  <si>
+    <t>https://www.myfirsthealth.com/LocateProvider/SelectNetworkType</t>
+  </si>
+  <si>
+    <t>First Health Coventry Website URL</t>
+  </si>
+  <si>
+    <t>Delta Dental Website URL</t>
+  </si>
+  <si>
+    <t>URL_UHRest</t>
+  </si>
+  <si>
+    <t>United Health Rest Website URL</t>
+  </si>
+  <si>
+    <t>URL_UHDental</t>
+  </si>
+  <si>
+    <t>United Health Dental Website URL</t>
   </si>
 </sst>
 </file>
@@ -954,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1059,73 +1080,69 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>176</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>113</v>
@@ -1136,7 +1153,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>113</v>
@@ -1147,7 +1164,7 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>113</v>
@@ -1158,10 +1175,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>111</v>
@@ -1169,7 +1186,7 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>113</v>
@@ -1180,7 +1197,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>113</v>
@@ -1191,7 +1208,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>113</v>
@@ -1200,9 +1217,39 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2171,13 +2218,16 @@
     <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A9:A19">
+  <conditionalFormatting sqref="A12:A22">
     <cfRule type="expression" dxfId="1" priority="11">
-      <formula>$B9="N"</formula>
+      <formula>$B12="N"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="12">
-      <formula>$B9="Y"</formula>
+      <formula>$B12="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UHC Rest Flow added and First Health Coventry Switch case renaming
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="183">
   <si>
     <t>Name</t>
   </si>
@@ -335,12 +335,6 @@
     <t>Blue Cross Blue Shield</t>
   </si>
   <si>
-    <t>Coventry Health Care</t>
-  </si>
-  <si>
-    <t>First Health (Coventry Health Care)</t>
-  </si>
-  <si>
     <t>PPO</t>
   </si>
   <si>
@@ -573,6 +567,9 @@
   </si>
   <si>
     <t>United Health Dental Website URL</t>
+  </si>
+  <si>
+    <t>First Health Coventry</t>
   </si>
 </sst>
 </file>
@@ -604,11 +601,13 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -975,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1025,10 +1024,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>45</v>
@@ -1058,64 +1057,64 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1134,10 +1133,10 @@
         <v>101</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1145,10 +1144,10 @@
         <v>102</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1156,100 +1155,90 @@
         <v>103</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2220,9 +2209,8 @@
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A12:A22">
+  <conditionalFormatting sqref="A12:A21">
     <cfRule type="expression" dxfId="1" priority="11">
       <formula>$B12="N"</formula>
     </cfRule>
@@ -2261,7 +2249,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2269,7 +2257,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2277,7 +2265,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2285,7 +2273,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2293,7 +2281,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2301,7 +2289,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2309,7 +2297,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2317,7 +2305,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2325,7 +2313,7 @@
         <v>58</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2333,7 +2321,7 @@
         <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2341,7 +2329,7 @@
         <v>60</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2349,7 +2337,7 @@
         <v>61</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2357,7 +2345,7 @@
         <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2365,7 +2353,7 @@
         <v>63</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2373,7 +2361,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2381,7 +2369,7 @@
         <v>65</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2389,7 +2377,7 @@
         <v>66</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2397,7 +2385,7 @@
         <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2405,7 +2393,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2413,7 +2401,7 @@
         <v>69</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2421,7 +2409,7 @@
         <v>70</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2429,7 +2417,7 @@
         <v>71</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2437,7 +2425,7 @@
         <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2445,7 +2433,7 @@
         <v>73</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2453,7 +2441,7 @@
         <v>74</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2461,7 +2449,7 @@
         <v>75</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2469,7 +2457,7 @@
         <v>76</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2477,7 +2465,7 @@
         <v>77</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2485,7 +2473,7 @@
         <v>78</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2493,7 +2481,7 @@
         <v>79</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2501,7 +2489,7 @@
         <v>80</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2509,7 +2497,7 @@
         <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2517,7 +2505,7 @@
         <v>82</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2525,7 +2513,7 @@
         <v>83</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2533,7 +2521,7 @@
         <v>84</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2541,7 +2529,7 @@
         <v>85</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2549,7 +2537,7 @@
         <v>86</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2557,7 +2545,7 @@
         <v>87</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2565,7 +2553,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2573,7 +2561,7 @@
         <v>89</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2581,7 +2569,7 @@
         <v>90</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2589,7 +2577,7 @@
         <v>91</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2597,7 +2585,7 @@
         <v>92</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2605,7 +2593,7 @@
         <v>93</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2613,7 +2601,7 @@
         <v>94</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2621,7 +2609,7 @@
         <v>95</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2629,7 +2617,7 @@
         <v>96</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2637,7 +2625,7 @@
         <v>97</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2645,7 +2633,7 @@
         <v>98</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2653,7 +2641,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2661,7 +2649,7 @@
         <v>100</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UnitedHealthCare Dental WF Added and Tested with Framework
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="185">
   <si>
     <t>Name</t>
   </si>
@@ -557,19 +557,25 @@
     <t>Delta Dental Website URL</t>
   </si>
   <si>
-    <t>URL_UHRest</t>
-  </si>
-  <si>
     <t>United Health Rest Website URL</t>
   </si>
   <si>
-    <t>URL_UHDental</t>
-  </si>
-  <si>
     <t>United Health Dental Website URL</t>
   </si>
   <si>
     <t>First Health Coventry</t>
+  </si>
+  <si>
+    <t>URL_UHCRest</t>
+  </si>
+  <si>
+    <t>URL_UHCDental</t>
+  </si>
+  <si>
+    <t>https://www.uhc.com/find-a-physician</t>
+  </si>
+  <si>
+    <t>https://connect.werally.com/state-plan-selection/uhc.medicaid/state</t>
   </si>
 </sst>
 </file>
@@ -976,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1101,20 +1107,24 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B10" s="7"/>
+        <v>182</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="C10" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1174,10 +1184,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>109</v>
@@ -1210,7 +1220,7 @@
         <v>106</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Anthem Plan extraction Issue Fixed using jscript
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1176,7 @@
         <v>108</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>109</v>
@@ -1220,7 +1220,7 @@
         <v>106</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
UHC Rest WF Development Completed Testing Remaining & Dublicate WebBranch Keywords Removed from List
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -983,7 +983,7 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1176,7 @@
         <v>108</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>109</v>
@@ -1231,7 +1231,7 @@
         <v>107</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
IP Change Functionality Added
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1143,7 @@
         <v>101</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>109</v>
@@ -1154,7 +1154,7 @@
         <v>102</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>109</v>
@@ -1187,7 +1187,7 @@
         <v>180</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>109</v>
@@ -1198,7 +1198,7 @@
         <v>104</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>109</v>
@@ -1209,7 +1209,7 @@
         <v>105</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>109</v>
@@ -1220,7 +1220,7 @@
         <v>106</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
MachineID added to error email, HMA is now work for Anthem and BCBS, HMA selector issue fixed
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="191">
   <si>
     <t>Name</t>
   </si>
@@ -401,9 +401,6 @@
     <t>Delaware</t>
   </si>
   <si>
-    <t>Dc</t>
-  </si>
-  <si>
     <t>Florida</t>
   </si>
   <si>
@@ -576,6 +573,27 @@
   </si>
   <si>
     <t>https://connect.werally.com/state-plan-selection/uhc.medicaid/state</t>
+  </si>
+  <si>
+    <t>Machine_ID</t>
+  </si>
+  <si>
+    <t>abcd1234</t>
+  </si>
+  <si>
+    <t>Email_To</t>
+  </si>
+  <si>
+    <t>satishc@damcogroup.com;satishsaggi007@gmail.com</t>
+  </si>
+  <si>
+    <t>damco.bot@gmail.com</t>
+  </si>
+  <si>
+    <t>Email_Cc</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
   </si>
 </sst>
 </file>
@@ -980,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1074,57 +1092,57 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>173</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1139,55 +1157,48 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>109</v>
-      </c>
+      <c r="A12" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="A13" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>109</v>
+      <c r="A14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>180</v>
+        <v>102</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>109</v>
@@ -1195,10 +1206,10 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>109</v>
@@ -1206,10 +1217,10 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>109</v>
@@ -1217,10 +1228,10 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>106</v>
+        <v>179</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>109</v>
@@ -1228,10 +1239,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>109</v>
@@ -1239,7 +1250,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>111</v>
@@ -1248,9 +1259,39 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2219,13 +2260,16 @@
     <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A12:A21">
+  <conditionalFormatting sqref="A15:A24">
     <cfRule type="expression" dxfId="1" priority="11">
-      <formula>$B12="N"</formula>
+      <formula>$B15="N"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="12">
-      <formula>$B12="Y"</formula>
+      <formula>$B15="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2238,7 +2282,7 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,7 +2367,7 @@
         <v>58</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2331,7 +2375,7 @@
         <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2339,7 +2383,7 @@
         <v>60</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2347,7 +2391,7 @@
         <v>61</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2355,7 +2399,7 @@
         <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2363,7 +2407,7 @@
         <v>63</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2371,7 +2415,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2379,7 +2423,7 @@
         <v>65</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2387,7 +2431,7 @@
         <v>66</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2395,7 +2439,7 @@
         <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2403,7 +2447,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2411,7 +2455,7 @@
         <v>69</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2419,7 +2463,7 @@
         <v>70</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2427,7 +2471,7 @@
         <v>71</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2435,7 +2479,7 @@
         <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2443,7 +2487,7 @@
         <v>73</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2451,7 +2495,7 @@
         <v>74</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2459,7 +2503,7 @@
         <v>75</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2467,7 +2511,7 @@
         <v>76</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2475,7 +2519,7 @@
         <v>77</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2483,7 +2527,7 @@
         <v>78</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2491,7 +2535,7 @@
         <v>79</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2499,7 +2543,7 @@
         <v>80</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2507,7 +2551,7 @@
         <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2515,7 +2559,7 @@
         <v>82</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2523,7 +2567,7 @@
         <v>83</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2531,7 +2575,7 @@
         <v>84</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2539,7 +2583,7 @@
         <v>85</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2547,7 +2591,7 @@
         <v>86</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2555,7 +2599,7 @@
         <v>87</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2563,7 +2607,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2571,7 +2615,7 @@
         <v>89</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2579,7 +2623,7 @@
         <v>90</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2587,7 +2631,7 @@
         <v>91</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2595,7 +2639,7 @@
         <v>92</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2603,7 +2647,7 @@
         <v>93</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2611,7 +2655,7 @@
         <v>94</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2619,7 +2663,7 @@
         <v>95</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2627,7 +2671,7 @@
         <v>96</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2635,7 +2679,7 @@
         <v>97</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2643,7 +2687,7 @@
         <v>98</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2651,7 +2695,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2659,7 +2703,7 @@
         <v>100</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced Excel Scope with Workbook activities for excel dependency removal, Resume functionality Added, Aetana Title Selector Issue Fixed, Browsing History Cleanup WF Added
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -1187,7 +1187,7 @@
         <v>101</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>109</v>
@@ -1275,7 +1275,7 @@
         <v>107</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
misouri pop up issue fix & custom error message for incorrect header placing in input file
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -356,244 +356,244 @@
     <t>Y</t>
   </si>
   <si>
+    <t>Delta Dental</t>
+  </si>
+  <si>
+    <t>URL_BCBS</t>
+  </si>
+  <si>
+    <t>https://provider.bcbs.com/app/public/#/one/city=&amp;state=&amp;postalCode=&amp;country=&amp;insurerCode=BCBSA_I&amp;brandCode=BCBSANDHF&amp;alphaPrefix=&amp;bcbsaProductId</t>
+  </si>
+  <si>
+    <t>URL_Anthem</t>
+  </si>
+  <si>
+    <t>https://www.anthem.com/health-insurance/providerreimagine-directory/searchcriteria?brand=ABCBS</t>
+  </si>
+  <si>
+    <t>Anthem Website URL</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>URL_Multiplan</t>
+  </si>
+  <si>
+    <t>https://www.multiplan.com/webcenter/portal/ProviderSearch?_afrLoop=4494409455183375&amp;_afrWindowMode=2&amp;Adf-Window-Id=g6y1unwep&amp;_afrFS=16&amp;_afrMT=screen&amp;_afrMFW=1366&amp;_afrMFH=576&amp;_afrMFDW=1366&amp;_afrMFDH=768&amp;_afrMFC=8&amp;_afrMFCI=0&amp;_afrMFM=0&amp;_afrMFR=96&amp;_afrMFG=0&amp;_afrMFS=0&amp;_afrMFO=0</t>
+  </si>
+  <si>
+    <t>Multiplan Website URL</t>
+  </si>
+  <si>
+    <t>URL_Delta</t>
+  </si>
+  <si>
+    <t>https://www.deltadentalins.com/find-a-dentist/directory-results/?d=enterprise&amp;network=2ppo&amp;location=2064%20Baldwin%20St;%20Ste%20A;%20Jenison;%20MI%2049428&amp;distance=15&amp;lat=42.9068881&amp;long=-85.8330607&amp;free_text=Vurugonda%20Anupama&amp;sort_field=relevance&amp;sort_order=asc&amp;isBookmarkedURL=false&amp;page=1</t>
+  </si>
+  <si>
+    <t>URL_Coventry</t>
+  </si>
+  <si>
+    <t>https://www.myfirsthealth.com/LocateProvider/SelectNetworkType</t>
+  </si>
+  <si>
+    <t>First Health Coventry Website URL</t>
+  </si>
+  <si>
+    <t>Delta Dental Website URL</t>
+  </si>
+  <si>
+    <t>United Health Rest Website URL</t>
+  </si>
+  <si>
+    <t>United Health Dental Website URL</t>
+  </si>
+  <si>
+    <t>First Health Coventry</t>
+  </si>
+  <si>
+    <t>URL_UHCRest</t>
+  </si>
+  <si>
+    <t>URL_UHCDental</t>
+  </si>
+  <si>
+    <t>https://www.uhc.com/find-a-physician</t>
+  </si>
+  <si>
+    <t>https://connect.werally.com/state-plan-selection/uhc.medicaid/state</t>
+  </si>
+  <si>
+    <t>Machine_ID</t>
+  </si>
+  <si>
+    <t>abcd1234</t>
+  </si>
+  <si>
+    <t>Email_To</t>
+  </si>
+  <si>
+    <t>satishc@damcogroup.com;satishsaggi007@gmail.com</t>
+  </si>
+  <si>
+    <t>Email_Cc</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>damco.bot@gmail.com;rawat.sandeep106@gmail.com</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Delta Dental</t>
-  </si>
-  <si>
-    <t>URL_BCBS</t>
-  </si>
-  <si>
-    <t>https://provider.bcbs.com/app/public/#/one/city=&amp;state=&amp;postalCode=&amp;country=&amp;insurerCode=BCBSA_I&amp;brandCode=BCBSANDHF&amp;alphaPrefix=&amp;bcbsaProductId</t>
-  </si>
-  <si>
-    <t>URL_Anthem</t>
-  </si>
-  <si>
-    <t>https://www.anthem.com/health-insurance/providerreimagine-directory/searchcriteria?brand=ABCBS</t>
-  </si>
-  <si>
-    <t>Anthem Website URL</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Alaska</t>
-  </si>
-  <si>
-    <t>Arizona</t>
-  </si>
-  <si>
-    <t>Arkansas</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Colorado</t>
-  </si>
-  <si>
-    <t>Connecticut</t>
-  </si>
-  <si>
-    <t>Delaware</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Georgia</t>
-  </si>
-  <si>
-    <t>Hawaii</t>
-  </si>
-  <si>
-    <t>Idaho</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>Kansas</t>
-  </si>
-  <si>
-    <t>Kentucky</t>
-  </si>
-  <si>
-    <t>Louisiana</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Massachusetts</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>Nebraska</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>New Hampshire</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>North Dakota</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>Oregon</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
-    <t>Rhode Island</t>
-  </si>
-  <si>
-    <t>South Carolina</t>
-  </si>
-  <si>
-    <t>South Dakota</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>Virginia</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>West Virginia</t>
-  </si>
-  <si>
-    <t>Wisconsin</t>
-  </si>
-  <si>
-    <t>Wyoming</t>
-  </si>
-  <si>
-    <t>URL_Multiplan</t>
-  </si>
-  <si>
-    <t>https://www.multiplan.com/webcenter/portal/ProviderSearch?_afrLoop=4494409455183375&amp;_afrWindowMode=2&amp;Adf-Window-Id=g6y1unwep&amp;_afrFS=16&amp;_afrMT=screen&amp;_afrMFW=1366&amp;_afrMFH=576&amp;_afrMFDW=1366&amp;_afrMFDH=768&amp;_afrMFC=8&amp;_afrMFCI=0&amp;_afrMFM=0&amp;_afrMFR=96&amp;_afrMFG=0&amp;_afrMFS=0&amp;_afrMFO=0</t>
-  </si>
-  <si>
-    <t>Multiplan Website URL</t>
-  </si>
-  <si>
-    <t>URL_Delta</t>
-  </si>
-  <si>
-    <t>https://www.deltadentalins.com/find-a-dentist/directory-results/?d=enterprise&amp;network=2ppo&amp;location=2064%20Baldwin%20St;%20Ste%20A;%20Jenison;%20MI%2049428&amp;distance=15&amp;lat=42.9068881&amp;long=-85.8330607&amp;free_text=Vurugonda%20Anupama&amp;sort_field=relevance&amp;sort_order=asc&amp;isBookmarkedURL=false&amp;page=1</t>
-  </si>
-  <si>
-    <t>URL_Coventry</t>
-  </si>
-  <si>
-    <t>https://www.myfirsthealth.com/LocateProvider/SelectNetworkType</t>
-  </si>
-  <si>
-    <t>First Health Coventry Website URL</t>
-  </si>
-  <si>
-    <t>Delta Dental Website URL</t>
-  </si>
-  <si>
-    <t>United Health Rest Website URL</t>
-  </si>
-  <si>
-    <t>United Health Dental Website URL</t>
-  </si>
-  <si>
-    <t>First Health Coventry</t>
-  </si>
-  <si>
-    <t>URL_UHCRest</t>
-  </si>
-  <si>
-    <t>URL_UHCDental</t>
-  </si>
-  <si>
-    <t>https://www.uhc.com/find-a-physician</t>
-  </si>
-  <si>
-    <t>https://connect.werally.com/state-plan-selection/uhc.medicaid/state</t>
-  </si>
-  <si>
-    <t>Machine_ID</t>
-  </si>
-  <si>
-    <t>abcd1234</t>
-  </si>
-  <si>
-    <t>Email_To</t>
-  </si>
-  <si>
-    <t>satishc@damcogroup.com;satishsaggi007@gmail.com</t>
-  </si>
-  <si>
-    <t>Email_Cc</t>
-  </si>
-  <si>
-    <t>District of Columbia</t>
-  </si>
-  <si>
-    <t>damco.bot@gmail.com;rawat.sandeep106@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1048,10 +1048,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>45</v>
@@ -1081,68 +1081,68 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>169</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>172</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>182</v>
-      </c>
       <c r="C10" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1158,28 +1158,28 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1187,7 +1187,7 @@
         <v>101</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>109</v>
@@ -1198,7 +1198,7 @@
         <v>102</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>109</v>
@@ -1209,7 +1209,7 @@
         <v>103</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>109</v>
@@ -1220,7 +1220,7 @@
         <v>108</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>109</v>
@@ -1228,10 +1228,10 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>109</v>
@@ -1242,7 +1242,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>109</v>
@@ -1253,7 +1253,7 @@
         <v>105</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>109</v>
@@ -1264,7 +1264,7 @@
         <v>106</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>109</v>
@@ -1275,7 +1275,7 @@
         <v>107</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>109</v>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>109</v>
@@ -2303,7 +2303,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2319,7 +2319,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2327,7 +2327,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2335,7 +2335,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2351,7 +2351,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>58</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
         <v>60</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2391,7 +2391,7 @@
         <v>61</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2399,7 +2399,7 @@
         <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
         <v>63</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2415,7 +2415,7 @@
         <v>64</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2423,7 +2423,7 @@
         <v>65</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2431,7 +2431,7 @@
         <v>66</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2447,7 +2447,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
         <v>69</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2463,7 +2463,7 @@
         <v>70</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>71</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,7 +2479,7 @@
         <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2487,7 @@
         <v>73</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
         <v>74</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
         <v>75</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,7 +2511,7 @@
         <v>76</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2519,7 +2519,7 @@
         <v>77</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2527,7 +2527,7 @@
         <v>78</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>79</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>80</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2551,7 +2551,7 @@
         <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>82</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>83</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,7 +2575,7 @@
         <v>84</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>85</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2591,7 +2591,7 @@
         <v>86</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2599,7 +2599,7 @@
         <v>87</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>88</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2615,7 +2615,7 @@
         <v>89</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2623,7 +2623,7 @@
         <v>90</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2631,7 +2631,7 @@
         <v>91</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>92</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2647,7 +2647,7 @@
         <v>93</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2655,7 +2655,7 @@
         <v>94</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2663,7 +2663,7 @@
         <v>95</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
         <v>96</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,7 +2679,7 @@
         <v>97</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,7 +2687,7 @@
         <v>98</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2703,7 +2703,7 @@
         <v>100</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2 sec Delay has been added to cigna prior Docto by name button click event
</commit_message>
<xml_diff>
--- a/Input/Config.xlsx
+++ b/Input/Config.xlsx
@@ -1001,7 +1001,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1198,7 @@
         <v>102</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>109</v>
@@ -1220,7 +1220,7 @@
         <v>108</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>109</v>

</xml_diff>